<commit_message>
AI input tab inexcel sheet
</commit_message>
<xml_diff>
--- a/be-estimation/template.xlsx
+++ b/be-estimation/template.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Projects\Estimation-rws\be-estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7B1DFD-AA05-488F-A0B9-D649633A3577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEEF526-FA9F-45A3-913E-1DE42304D565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
     <sheet name="Schedule" sheetId="2" r:id="rId2"/>
     <sheet name="Technology Stack" sheetId="7" r:id="rId3"/>
     <sheet name="Assumption &amp; Queries" sheetId="5" r:id="rId4"/>
+    <sheet name="AI Input" sheetId="8" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WBS!$B$6:$F$95</definedName>
@@ -44,6 +45,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -676,7 +699,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -901,6 +924,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -910,23 +936,26 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1119,6 +1148,70 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2122,7 +2215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61ACB7D-6544-40FF-87F9-22A62379963A}">
   <dimension ref="B2:I12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -2141,13 +2234,13 @@
     <row r="2" spans="2:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="76"/>
       <c r="C2" s="76"/>
-      <c r="D2" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="D2" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -2158,63 +2251,63 @@
       </c>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="79"/>
-      <c r="H3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="81"/>
       <c r="I3" s="32"/>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
       <c r="I4" s="32"/>
     </row>
     <row r="5" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
       <c r="I5" s="32"/>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
       <c r="I6" s="32"/>
     </row>
     <row r="7" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
       <c r="I7" s="32"/>
     </row>
     <row r="8" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
       <c r="I8" s="32"/>
     </row>
     <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2249,6 +2342,119 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B9FD0D-73C5-4B9E-B1AB-57E380CE35A3}">
+  <sheetPr>
+    <tabColor theme="6"/>
+  </sheetPr>
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="57.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="0.5546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="3.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="87" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="88"/>
+      <c r="B2" s="88"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="88"/>
+      <c r="B3" s="88"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="88"/>
+      <c r="B4" s="88"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="88"/>
+      <c r="B5" s="88"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="88"/>
+      <c r="B6" s="88"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="88"/>
+      <c r="B7" s="88"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="88"/>
+      <c r="B8" s="88"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="88"/>
+      <c r="B9" s="88"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="88"/>
+      <c r="B10" s="88"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="88"/>
+      <c r="B13" s="88"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="88"/>
+      <c r="B14" s="88"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="88"/>
+      <c r="B15" s="88"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="88"/>
+      <c r="B16" s="88"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="88"/>
+      <c r="B17" s="88"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="88"/>
+      <c r="B18" s="88"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="88"/>
+      <c r="B19" s="88"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:B19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Scheudler phase - 1 (D3.26)
</commit_message>
<xml_diff>
--- a/be-estimation/template.xlsx
+++ b/be-estimation/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Projects\Estimation-rws\be-estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E177C46-8371-4105-8A79-DECF1F5E9C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E586BC-98B9-418C-9C00-F599C2D165F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>RWS India Private Limited</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Development</t>
+  </si>
+  <si>
+    <t>Hours Per week</t>
   </si>
 </sst>
 </file>
@@ -203,7 +206,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot; $&quot;#,##0.00\ ;&quot; $(&quot;#,##0.00\);&quot; $-&quot;#\ ;@\ "/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,8 +369,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,8 +463,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -690,6 +707,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -699,7 +727,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -803,9 +831,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -827,6 +852,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -881,35 +910,35 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -956,6 +985,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1519,19 +1566,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:39" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="58"/>
       <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="4" spans="1:39" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="55"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="28"/>
     </row>
     <row r="6" spans="1:39" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
@@ -1593,20 +1640,20 @@
       <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="11"/>
       <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="B9" s="45"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="47"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="48"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
@@ -1649,18 +1696,18 @@
       <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="48"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="54"/>
       <c r="E15" s="13">
         <f>ROUND(SUM(E8,E10:E13),0)</f>
         <v>0</v>
@@ -1733,10 +1780,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:Q13"/>
+  <dimension ref="A2:R13"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:K10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1745,53 +1792,55 @@
     <col min="2" max="2" width="28.5546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="1.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="2"/>
-    <col min="6" max="14" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="2"/>
+    <col min="5" max="6" width="9.109375" style="2"/>
+    <col min="7" max="15" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33"/>
-      <c r="B2" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="33"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F3" s="34"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+    </row>
+    <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="33"/>
       <c r="B4" s="66" t="s">
         <v>23</v>
@@ -1799,69 +1848,71 @@
       <c r="C4" s="66"/>
       <c r="D4" s="33"/>
       <c r="E4" s="33"/>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="H4" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="44" t="s">
+      <c r="I4" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="J4" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="44" t="s">
+      <c r="K4" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="44" t="s">
+      <c r="L4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="44" t="s">
+      <c r="M4" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="44" t="s">
+      <c r="N4" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="44" t="s">
+      <c r="O4" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="44" t="s">
+      <c r="P4" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="44" t="s">
+      <c r="Q4" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="44" t="s">
+      <c r="R4" s="43" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="33"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
-      <c r="F5" s="67" t="s">
+      <c r="F5" s="91"/>
+      <c r="G5" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="68"/>
       <c r="H5" s="68"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70" t="s">
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="68"/>
       <c r="L5" s="68"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="70" t="s">
+      <c r="M5" s="68"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="68"/>
       <c r="P5" s="68"/>
-      <c r="Q5" s="69"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q5" s="68"/>
+      <c r="R5" s="69"/>
+    </row>
+    <row r="6" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>15</v>
       </c>
@@ -1870,13 +1921,15 @@
         <v>6</v>
       </c>
       <c r="D6" s="72"/>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="64" t="s">
+      <c r="G6" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="65"/>
       <c r="H6" s="65"/>
       <c r="I6" s="65"/>
       <c r="J6" s="65"/>
@@ -1887,269 +1940,288 @@
       <c r="O6" s="65"/>
       <c r="P6" s="65"/>
       <c r="Q6" s="65"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="38">
+      <c r="R6" s="65"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="37">
         <v>1</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="40">
-        <f>SUM(F7:Q7)</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="41">
-        <v>0</v>
-      </c>
-      <c r="G7" s="41">
-        <v>0</v>
-      </c>
-      <c r="H7" s="41">
-        <v>0</v>
-      </c>
-      <c r="I7" s="41">
-        <v>0</v>
-      </c>
-      <c r="J7" s="41">
-        <v>0</v>
-      </c>
-      <c r="K7" s="41">
-        <v>0</v>
-      </c>
-      <c r="L7" s="41">
-        <v>0</v>
-      </c>
-      <c r="M7" s="41">
-        <v>0</v>
-      </c>
-      <c r="N7" s="41">
-        <v>0</v>
-      </c>
-      <c r="O7" s="41">
-        <v>0</v>
-      </c>
-      <c r="P7" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="38">
+      <c r="B7" s="38"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="39">
+        <f>SUM(G7:R7)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="95">
+        <f>(SUM(G7:R7)*5)/8</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="94">
+        <v>0</v>
+      </c>
+      <c r="H7" s="40">
+        <v>0</v>
+      </c>
+      <c r="I7" s="40">
+        <v>0</v>
+      </c>
+      <c r="J7" s="40">
+        <v>0</v>
+      </c>
+      <c r="K7" s="40">
+        <v>0</v>
+      </c>
+      <c r="L7" s="40">
+        <v>0</v>
+      </c>
+      <c r="M7" s="40">
+        <v>0</v>
+      </c>
+      <c r="N7" s="40">
+        <v>0</v>
+      </c>
+      <c r="O7" s="40">
+        <v>0</v>
+      </c>
+      <c r="P7" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="40">
+        <v>0</v>
+      </c>
+      <c r="R7" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="37">
         <v>2</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="40">
-        <f t="shared" ref="E8:E9" si="0">SUM(F8:Q8)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="41">
-        <v>0</v>
-      </c>
-      <c r="G8" s="41">
-        <v>0</v>
-      </c>
-      <c r="H8" s="41">
-        <v>0</v>
-      </c>
-      <c r="I8" s="41">
-        <v>0</v>
-      </c>
-      <c r="J8" s="41">
-        <v>0</v>
-      </c>
-      <c r="K8" s="41">
-        <v>0</v>
-      </c>
-      <c r="L8" s="41">
-        <v>0</v>
-      </c>
-      <c r="M8" s="41">
-        <v>0</v>
-      </c>
-      <c r="N8" s="41">
-        <v>0</v>
-      </c>
-      <c r="O8" s="41">
-        <v>0</v>
-      </c>
-      <c r="P8" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="38">
+      <c r="B8" s="41"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="39">
+        <f t="shared" ref="E8:E9" si="0">SUM(G8:R8)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="95">
+        <f t="shared" ref="F8:F9" si="1">(SUM(G8:R8)*5)/8</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="94">
+        <v>0</v>
+      </c>
+      <c r="H8" s="40">
+        <v>0</v>
+      </c>
+      <c r="I8" s="40">
+        <v>0</v>
+      </c>
+      <c r="J8" s="40">
+        <v>0</v>
+      </c>
+      <c r="K8" s="40">
+        <v>0</v>
+      </c>
+      <c r="L8" s="40">
+        <v>0</v>
+      </c>
+      <c r="M8" s="40">
+        <v>0</v>
+      </c>
+      <c r="N8" s="40">
+        <v>0</v>
+      </c>
+      <c r="O8" s="40">
+        <v>0</v>
+      </c>
+      <c r="P8" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="40">
+        <v>0</v>
+      </c>
+      <c r="R8" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="37">
         <v>3</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="40">
+      <c r="B9" s="42"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="41">
-        <v>0</v>
-      </c>
-      <c r="G9" s="41">
-        <v>0</v>
-      </c>
-      <c r="H9" s="41">
-        <v>0</v>
-      </c>
-      <c r="I9" s="41">
-        <v>0</v>
-      </c>
-      <c r="J9" s="41">
-        <v>0</v>
-      </c>
-      <c r="K9" s="41">
-        <v>0</v>
-      </c>
-      <c r="L9" s="41">
-        <v>0</v>
-      </c>
-      <c r="M9" s="41">
-        <v>0</v>
-      </c>
-      <c r="N9" s="41">
-        <v>0</v>
-      </c>
-      <c r="O9" s="41">
-        <v>0</v>
-      </c>
-      <c r="P9" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="95">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="94">
+        <v>0</v>
+      </c>
+      <c r="H9" s="40">
+        <v>0</v>
+      </c>
+      <c r="I9" s="40">
+        <v>0</v>
+      </c>
+      <c r="J9" s="40">
+        <v>0</v>
+      </c>
+      <c r="K9" s="40">
+        <v>0</v>
+      </c>
+      <c r="L9" s="40">
+        <v>0</v>
+      </c>
+      <c r="M9" s="40">
+        <v>0</v>
+      </c>
+      <c r="N9" s="40">
+        <v>0</v>
+      </c>
+      <c r="O9" s="40">
+        <v>0</v>
+      </c>
+      <c r="P9" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="40">
+        <v>0</v>
+      </c>
+      <c r="R9" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33"/>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="63"/>
-      <c r="P10" s="63"/>
-      <c r="Q10" s="63"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="E10" s="93">
+        <f>SUM(E7:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="93">
+        <f>SUM(F7:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="58"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="59"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="59"/>
+      <c r="R12" s="59"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="33"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="58"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="59"/>
+      <c r="R13" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="C6:D6"/>
+  <mergeCells count="36">
+    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F6:Q6"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="G6:R6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2176,11 +2248,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
@@ -2232,82 +2304,82 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="86" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="79" t="s">
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="80"/>
-      <c r="H3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="82"/>
       <c r="I3" s="32"/>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
       <c r="I4" s="32"/>
     </row>
     <row r="5" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
       <c r="I5" s="32"/>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
       <c r="I6" s="32"/>
     </row>
     <row r="7" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
       <c r="I7" s="32"/>
     </row>
     <row r="8" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
       <c r="I8" s="32"/>
     </row>
     <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2352,7 +2424,7 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -2367,87 +2439,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="e" vm="1">
+      <c r="A1" s="88" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="88"/>
-      <c r="B2" s="88"/>
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="88"/>
-      <c r="B3" s="88"/>
+      <c r="A3" s="89"/>
+      <c r="B3" s="89"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="88"/>
-      <c r="B4" s="88"/>
+      <c r="A4" s="89"/>
+      <c r="B4" s="89"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
-      <c r="B5" s="88"/>
+      <c r="A5" s="89"/>
+      <c r="B5" s="89"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="88"/>
-      <c r="B6" s="88"/>
+      <c r="A6" s="89"/>
+      <c r="B6" s="89"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
-      <c r="B7" s="88"/>
+      <c r="A7" s="89"/>
+      <c r="B7" s="89"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="88"/>
-      <c r="B8" s="88"/>
+      <c r="A8" s="89"/>
+      <c r="B8" s="89"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="88"/>
-      <c r="B9" s="88"/>
+      <c r="A9" s="89"/>
+      <c r="B9" s="89"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="88"/>
-      <c r="B10" s="88"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="88"/>
-      <c r="B11" s="88"/>
+      <c r="A11" s="89"/>
+      <c r="B11" s="89"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="88"/>
-      <c r="B12" s="88"/>
+      <c r="A12" s="89"/>
+      <c r="B12" s="89"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
+      <c r="A13" s="89"/>
+      <c r="B13" s="89"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="88"/>
-      <c r="B14" s="88"/>
+      <c r="A14" s="89"/>
+      <c r="B14" s="89"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
-      <c r="B15" s="88"/>
+      <c r="A15" s="89"/>
+      <c r="B15" s="89"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="88"/>
-      <c r="B16" s="88"/>
+      <c r="A16" s="89"/>
+      <c r="B16" s="89"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="88"/>
-      <c r="B17" s="88"/>
+      <c r="A17" s="89"/>
+      <c r="B17" s="89"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="88"/>
-      <c r="B18" s="88"/>
+      <c r="A18" s="89"/>
+      <c r="B18" s="89"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="88"/>
-      <c r="B19" s="88"/>
+      <c r="A19" s="89"/>
+      <c r="B19" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2459,17 +2531,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizIdPermissions xmlns="c73d9a9f-9dfd-4531-9cef-cecd81e19837" xsi:nil="true"/>
-    <_activity xmlns="c73d9a9f-9dfd-4531-9cef-cecd81e19837" xsi:nil="true"/>
-    <MigrationWizId xmlns="c73d9a9f-9dfd-4531-9cef-cecd81e19837" xsi:nil="true"/>
-    <MigrationWizIdVersion xmlns="c73d9a9f-9dfd-4531-9cef-cecd81e19837" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006194F9D8A7FF7F4D9CE277BD2313E3F3" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1db5c6dda6608ad6f2420652cbe17304">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c73d9a9f-9dfd-4531-9cef-cecd81e19837" xmlns:ns4="edc975c7-0914-457f-802e-851999ba342c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b9281b5c0eac46c82836c40b4a94ab06" ns3:_="" ns4:_="">
     <xsd:import namespace="c73d9a9f-9dfd-4531-9cef-cecd81e19837"/>
@@ -2720,7 +2781,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2729,17 +2790,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79F69EEA-0D4B-406A-B1FD-F5EED703C937}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c73d9a9f-9dfd-4531-9cef-cecd81e19837"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizIdPermissions xmlns="c73d9a9f-9dfd-4531-9cef-cecd81e19837" xsi:nil="true"/>
+    <_activity xmlns="c73d9a9f-9dfd-4531-9cef-cecd81e19837" xsi:nil="true"/>
+    <MigrationWizId xmlns="c73d9a9f-9dfd-4531-9cef-cecd81e19837" xsi:nil="true"/>
+    <MigrationWizIdVersion xmlns="c73d9a9f-9dfd-4531-9cef-cecd81e19837" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA5FC516-3930-4809-8DA2-4D754101E02F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2758,10 +2820,20 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBB736AE-332F-4AD2-B4B0-7E0B0BF50609}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79F69EEA-0D4B-406A-B1FD-F5EED703C937}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c73d9a9f-9dfd-4531-9cef-cecd81e19837"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>